<commit_message>
charts and figures updated
</commit_message>
<xml_diff>
--- a/EJBComponents/ImageProcessingBenchmark_3/stats/ExcelSheets/ImagePreparationTimes.xlsx
+++ b/EJBComponents/ImageProcessingBenchmark_3/stats/ExcelSheets/ImagePreparationTimes.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\CourseWork\GitHubRepositories\CloudComputingComponents\CloudComputingComponents\EJBComponents\ImageProcessingBenchmark_3\stats\PowerConsumption\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="11865" yWindow="-15" windowWidth="16950" windowHeight="14805"/>
   </bookViews>
@@ -32,7 +27,7 @@
     <externalReference r:id="rId16"/>
     <externalReference r:id="rId17"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -246,6 +241,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -255,6 +259,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -262,18 +269,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -305,7 +300,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-NZ"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -337,7 +332,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-NZ" sz="1600" b="1" baseline="0"/>
-              <a:t>Preparation Time of Images </a:t>
+              <a:t>Preparation Time of Images - Local Mode </a:t>
             </a:r>
             <a:endParaRPr lang="en-NZ" sz="1600" b="1"/>
           </a:p>
@@ -347,8 +342,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37810445442176072"/>
-          <c:y val="7.1905501450283005E-3"/>
+          <c:x val="0.32426592329152504"/>
+          <c:y val="5.7524401160226404E-3"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -359,26 +354,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1226,1291 +1201,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="363766672"/>
-        <c:axId val="363769392"/>
+        <c:axId val="108288640"/>
+        <c:axId val="108311680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="363766672"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="90000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-NZ" sz="1600"/>
-                  <a:t>Number</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-NZ" sz="1600" baseline="0"/>
-                  <a:t> of Sub-Images</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-NZ" sz="1600"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.43387804537243624"/>
-              <c:y val="0.96759938104650245"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="65000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="363769392"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="363769392"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="22"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-NZ" sz="1600"/>
-                  <a:t>Time </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-NZ" sz="1600" baseline="0"/>
-                  <a:t>(Minutes)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-NZ" sz="1600"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="6.4828350310221921E-4"/>
-              <c:y val="0.38225474137516158"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="bg1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="363766672"/>
-        <c:crossesAt val="1"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="2"/>
-        <c:minorUnit val="0.5"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.41464322484119426"/>
-          <c:y val="5.7441851379821281E-2"/>
-          <c:w val="0.56783898715113734"/>
-          <c:h val="5.7527118848470206E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-NZ" sz="1600" b="1" baseline="0"/>
-              <a:t>Preparation Time of Images </a:t>
-            </a:r>
-            <a:endParaRPr lang="en-NZ" sz="1600" b="1"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.37810445442176072"/>
-          <c:y val="7.1905501450283005E-3"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="7.0417757672607162E-2"/>
-          <c:y val="5.273289031240392E-2"/>
-          <c:w val="0.90510744663137499"/>
-          <c:h val="0.88659981531043641"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>OneThread_Remote</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="10"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="12700">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$38:$J$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$7:$J$7</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>3.7638500000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.8110833333333334</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.069</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.0624166666666666</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.7954666666666665</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.7473999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.7686000000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.9925833333333332</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.7668166666666667</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>TwoThreads_Remote</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="10"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="12700">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$38:$J$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$12:$J$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>3.8550499999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.9191499999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5183666666666666</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.8713666666666666</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.8687833333333332</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.8672166666666667</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.8671833333333334</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.8769666666666667</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.8753500000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>ThreeThreads_Remote</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="10"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="12700">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$38:$J$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$17:$J$17</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>4.3458833333333331</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.9641333333333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.9232166666666666</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2758666666666667</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.4263166666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.5261499999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.2783666666666667</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.3669666666666667</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.4297166666666667</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>FourThreads_Remote</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="10"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="12700">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$38:$J$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$22:$J$22</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>4.3445</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.9661166666666667</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.94664999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2753666666666668</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.96260000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1440666666666666</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.95979999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.08785</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.78249999999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:v>FiveThreads_Remote</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:prstDash val="dash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="10"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="12700">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$38:$J$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$27:$J$27</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>3.8630333333333335</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.9161333333333332</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.96935000000000004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.4045833333333333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.87186666666666668</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0323166666666668</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0924166666666666</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.98866666666666669</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.90669999999999995</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="11"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:v>SixThreads_Remote</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:prstDash val="dash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="10"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="12700">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$38:$J$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$32:$J$32</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>3.7638333333333334</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.9193499999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.94618333333333338</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.99721666666666664</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1727833333333333</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.96838333333333337</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.81181666666666663</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0661666666666667</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.9750833333333333</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="13"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:v>SevenThreads_Remote</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:prstDash val="dash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="10"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="12700">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$38:$J$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$37:$J$37</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>3.8622166666666669</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.96435</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.94668333333333332</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0125166666666667</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.2851166666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0445833333333334</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.98819999999999997</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.98183333333333334</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.0482333333333334</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="15"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:v>EightThreads_Remote</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:prstDash val="dash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="10"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="12700">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$38:$J$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$42:$J$42</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>4.3433999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.9130666666666667</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.94561666666666666</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.98358333333333337</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.81706666666666672</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1251333333333333</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.78576666666666661</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.81541666666666668</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.98570000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="363769936"/>
-        <c:axId val="363772656"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="363769936"/>
+        <c:axId val="108288640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2626,7 +1321,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363772656"/>
+        <c:crossAx val="108311680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2634,7 +1329,1247 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="363772656"/>
+        <c:axId val="108311680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="22"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ" sz="1600"/>
+                  <a:t>Time </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" sz="1600" baseline="0"/>
+                  <a:t>(Minutes)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="6.4828350310221921E-4"/>
+              <c:y val="0.38225474137516158"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="108288640"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+        <c:minorUnit val="0.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.41464322484119426"/>
+          <c:y val="5.7441851379821281E-2"/>
+          <c:w val="0.56783898715113734"/>
+          <c:h val="5.7527118848470206E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-NZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ" sz="1600" b="1" baseline="0"/>
+              <a:t>Preparation Time of Images - Remote Mode </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-NZ" sz="1600" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.33177828171265211"/>
+          <c:y val="2.8762200580113202E-3"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.0417757672607162E-2"/>
+          <c:y val="5.273289031240392E-2"/>
+          <c:w val="0.90510744663137499"/>
+          <c:h val="0.88659981531043641"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>OneThread_Remote</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$38:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.7638500000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8110833333333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.069</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0624166666666666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7954666666666665</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7473999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.7686000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9925833333333332</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7668166666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>TwoThreads_Remote</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$38:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.8550499999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9191499999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5183666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8713666666666666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8687833333333332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8672166666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8671833333333334</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8769666666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8753500000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>ThreeThreads_Remote</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$38:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$17:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.3458833333333331</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9641333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9232166666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2758666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4263166666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5261499999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2783666666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3669666666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4297166666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>FourThreads_Remote</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$38:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$22:$J$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.3445</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9661166666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94664999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2753666666666668</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96260000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1440666666666666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.95979999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.08785</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.78249999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>FiveThreads_Remote</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$38:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$27:$J$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.8630333333333335</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9161333333333332</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96935000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4045833333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.87186666666666668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0323166666666668</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0924166666666666</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98866666666666669</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.90669999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>SixThreads_Remote</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$38:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$32:$J$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.7638333333333334</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9193499999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94618333333333338</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99721666666666664</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1727833333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96838333333333337</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.81181666666666663</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0661666666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9750833333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>SevenThreads_Remote</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$38:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$37:$J$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.8622166666666669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.96435</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94668333333333332</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0125166666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2851166666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0445833333333334</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98819999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98183333333333334</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0482333333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>EightThreads_Remote</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$38:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$42:$J$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.3433999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9130666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94561666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98358333333333337</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81706666666666672</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1251333333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.78576666666666661</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.81541666666666668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.98570000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="111909504"/>
+        <c:axId val="111924352"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="111909504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ" sz="1600"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" sz="1600" baseline="0"/>
+                  <a:t> of Sub-Images</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.43387804537243624"/>
+              <c:y val="0.96759938104650245"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="111924352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="111924352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22"/>
@@ -2749,7 +2684,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363769936"/>
+        <c:crossAx val="111909504"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -2844,7 +2779,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-NZ"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3888,11 +3823,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="359866016"/>
-        <c:axId val="359870912"/>
+        <c:axId val="112230400"/>
+        <c:axId val="112232704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359866016"/>
+        <c:axId val="112230400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4003,7 +3938,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359870912"/>
+        <c:crossAx val="112232704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4011,7 +3946,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359870912"/>
+        <c:axId val="112232704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="48"/>
@@ -4126,7 +4061,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359866016"/>
+        <c:crossAx val="112230400"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4"/>
@@ -4221,7 +4156,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-NZ"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5265,11 +5200,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="359538272"/>
-        <c:axId val="157894096"/>
+        <c:axId val="112345856"/>
+        <c:axId val="112348160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359538272"/>
+        <c:axId val="112345856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5380,7 +5315,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157894096"/>
+        <c:crossAx val="112348160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5388,7 +5323,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="157894096"/>
+        <c:axId val="112348160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="48"/>
@@ -5503,7 +5438,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359538272"/>
+        <c:crossAx val="112345856"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4"/>
@@ -7227,7 +7162,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9330,41 +9265,41 @@
       </c>
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A59" s="21" t="s">
+      <c r="A59" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
-      <c r="G59" s="21"/>
-      <c r="H59" s="21"/>
-      <c r="I59" s="21"/>
-      <c r="J59" s="21"/>
-      <c r="K59" s="21"/>
-      <c r="L59" s="21"/>
-      <c r="M59" s="21"/>
-      <c r="N59" s="21"/>
-      <c r="O59" s="21"/>
-      <c r="P59" s="21"/>
-      <c r="Q59" s="21"/>
-      <c r="R59" s="21"/>
-      <c r="S59" s="21"/>
-      <c r="T59" s="21"/>
-      <c r="U59" s="21"/>
-      <c r="V59" s="21"/>
-      <c r="W59" s="21"/>
-      <c r="X59" s="21"/>
-      <c r="Y59" s="21"/>
-      <c r="Z59" s="21"/>
-      <c r="AA59" s="21"/>
-      <c r="AB59" s="21"/>
-      <c r="AC59" s="21"/>
-      <c r="AD59" s="21"/>
-      <c r="AE59" s="21"/>
-      <c r="AF59" s="21"/>
-      <c r="AG59" s="21"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="18"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="18"/>
+      <c r="L59" s="18"/>
+      <c r="M59" s="18"/>
+      <c r="N59" s="18"/>
+      <c r="O59" s="18"/>
+      <c r="P59" s="18"/>
+      <c r="Q59" s="18"/>
+      <c r="R59" s="18"/>
+      <c r="S59" s="18"/>
+      <c r="T59" s="18"/>
+      <c r="U59" s="18"/>
+      <c r="V59" s="18"/>
+      <c r="W59" s="18"/>
+      <c r="X59" s="18"/>
+      <c r="Y59" s="18"/>
+      <c r="Z59" s="18"/>
+      <c r="AA59" s="18"/>
+      <c r="AB59" s="18"/>
+      <c r="AC59" s="18"/>
+      <c r="AD59" s="18"/>
+      <c r="AE59" s="18"/>
+      <c r="AF59" s="18"/>
+      <c r="AG59" s="18"/>
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
@@ -9959,78 +9894,78 @@
       </c>
     </row>
     <row r="66" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A66" s="15" t="s">
+      <c r="A66" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="16"/>
-      <c r="I66" s="16"/>
-      <c r="J66" s="16"/>
-      <c r="K66" s="16"/>
-      <c r="L66" s="16"/>
-      <c r="M66" s="16"/>
-      <c r="N66" s="16"/>
-      <c r="O66" s="16"/>
-      <c r="P66" s="16"/>
-      <c r="Q66" s="16"/>
-      <c r="R66" s="16"/>
-      <c r="S66" s="16"/>
-      <c r="T66" s="16"/>
-      <c r="U66" s="16"/>
-      <c r="V66" s="16"/>
-      <c r="W66" s="16"/>
-      <c r="X66" s="16"/>
-      <c r="Y66" s="16"/>
-      <c r="Z66" s="16"/>
-      <c r="AA66" s="16"/>
-      <c r="AB66" s="16"/>
-      <c r="AC66" s="16"/>
-      <c r="AD66" s="16"/>
-      <c r="AE66" s="16"/>
-      <c r="AF66" s="16"/>
-      <c r="AG66" s="17"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="20"/>
+      <c r="I66" s="20"/>
+      <c r="J66" s="20"/>
+      <c r="K66" s="20"/>
+      <c r="L66" s="20"/>
+      <c r="M66" s="20"/>
+      <c r="N66" s="20"/>
+      <c r="O66" s="20"/>
+      <c r="P66" s="20"/>
+      <c r="Q66" s="20"/>
+      <c r="R66" s="20"/>
+      <c r="S66" s="20"/>
+      <c r="T66" s="20"/>
+      <c r="U66" s="20"/>
+      <c r="V66" s="20"/>
+      <c r="W66" s="20"/>
+      <c r="X66" s="20"/>
+      <c r="Y66" s="20"/>
+      <c r="Z66" s="20"/>
+      <c r="AA66" s="20"/>
+      <c r="AB66" s="20"/>
+      <c r="AC66" s="20"/>
+      <c r="AD66" s="20"/>
+      <c r="AE66" s="20"/>
+      <c r="AF66" s="20"/>
+      <c r="AG66" s="21"/>
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A67" s="18" t="s">
+      <c r="A67" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B67" s="19"/>
-      <c r="C67" s="19"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="19"/>
-      <c r="G67" s="19"/>
-      <c r="H67" s="19"/>
-      <c r="I67" s="19"/>
-      <c r="J67" s="19"/>
-      <c r="K67" s="19"/>
-      <c r="L67" s="19"/>
-      <c r="M67" s="19"/>
-      <c r="N67" s="19"/>
-      <c r="O67" s="19"/>
-      <c r="P67" s="19"/>
-      <c r="Q67" s="19"/>
-      <c r="R67" s="19"/>
-      <c r="S67" s="19"/>
-      <c r="T67" s="19"/>
-      <c r="U67" s="19"/>
-      <c r="V67" s="19"/>
-      <c r="W67" s="19"/>
-      <c r="X67" s="19"/>
-      <c r="Y67" s="19"/>
-      <c r="Z67" s="19"/>
-      <c r="AA67" s="19"/>
-      <c r="AB67" s="19"/>
-      <c r="AC67" s="19"/>
-      <c r="AD67" s="19"/>
-      <c r="AE67" s="19"/>
-      <c r="AF67" s="19"/>
-      <c r="AG67" s="20"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13"/>
+      <c r="M67" s="13"/>
+      <c r="N67" s="13"/>
+      <c r="O67" s="13"/>
+      <c r="P67" s="13"/>
+      <c r="Q67" s="13"/>
+      <c r="R67" s="13"/>
+      <c r="S67" s="13"/>
+      <c r="T67" s="13"/>
+      <c r="U67" s="13"/>
+      <c r="V67" s="13"/>
+      <c r="W67" s="13"/>
+      <c r="X67" s="13"/>
+      <c r="Y67" s="13"/>
+      <c r="Z67" s="13"/>
+      <c r="AA67" s="13"/>
+      <c r="AB67" s="13"/>
+      <c r="AC67" s="13"/>
+      <c r="AD67" s="13"/>
+      <c r="AE67" s="13"/>
+      <c r="AF67" s="13"/>
+      <c r="AG67" s="14"/>
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
@@ -10625,41 +10560,41 @@
       </c>
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A74" s="12" t="s">
+      <c r="A74" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="13"/>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
-      <c r="K74" s="13"/>
-      <c r="L74" s="13"/>
-      <c r="M74" s="13"/>
-      <c r="N74" s="13"/>
-      <c r="O74" s="13"/>
-      <c r="P74" s="13"/>
-      <c r="Q74" s="13"/>
-      <c r="R74" s="13"/>
-      <c r="S74" s="13"/>
-      <c r="T74" s="13"/>
-      <c r="U74" s="13"/>
-      <c r="V74" s="13"/>
-      <c r="W74" s="13"/>
-      <c r="X74" s="13"/>
-      <c r="Y74" s="13"/>
-      <c r="Z74" s="13"/>
-      <c r="AA74" s="13"/>
-      <c r="AB74" s="13"/>
-      <c r="AC74" s="13"/>
-      <c r="AD74" s="13"/>
-      <c r="AE74" s="13"/>
-      <c r="AF74" s="13"/>
-      <c r="AG74" s="14"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="16"/>
+      <c r="L74" s="16"/>
+      <c r="M74" s="16"/>
+      <c r="N74" s="16"/>
+      <c r="O74" s="16"/>
+      <c r="P74" s="16"/>
+      <c r="Q74" s="16"/>
+      <c r="R74" s="16"/>
+      <c r="S74" s="16"/>
+      <c r="T74" s="16"/>
+      <c r="U74" s="16"/>
+      <c r="V74" s="16"/>
+      <c r="W74" s="16"/>
+      <c r="X74" s="16"/>
+      <c r="Y74" s="16"/>
+      <c r="Z74" s="16"/>
+      <c r="AA74" s="16"/>
+      <c r="AB74" s="16"/>
+      <c r="AC74" s="16"/>
+      <c r="AD74" s="16"/>
+      <c r="AE74" s="16"/>
+      <c r="AF74" s="16"/>
+      <c r="AG74" s="17"/>
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
@@ -11254,78 +11189,78 @@
       </c>
     </row>
     <row r="83" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A83" s="15" t="s">
+      <c r="A83" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B83" s="16"/>
-      <c r="C83" s="16"/>
-      <c r="D83" s="16"/>
-      <c r="E83" s="16"/>
-      <c r="F83" s="16"/>
-      <c r="G83" s="16"/>
-      <c r="H83" s="16"/>
-      <c r="I83" s="16"/>
-      <c r="J83" s="16"/>
-      <c r="K83" s="16"/>
-      <c r="L83" s="16"/>
-      <c r="M83" s="16"/>
-      <c r="N83" s="16"/>
-      <c r="O83" s="16"/>
-      <c r="P83" s="16"/>
-      <c r="Q83" s="16"/>
-      <c r="R83" s="16"/>
-      <c r="S83" s="16"/>
-      <c r="T83" s="16"/>
-      <c r="U83" s="16"/>
-      <c r="V83" s="16"/>
-      <c r="W83" s="16"/>
-      <c r="X83" s="16"/>
-      <c r="Y83" s="16"/>
-      <c r="Z83" s="16"/>
-      <c r="AA83" s="16"/>
-      <c r="AB83" s="16"/>
-      <c r="AC83" s="16"/>
-      <c r="AD83" s="16"/>
-      <c r="AE83" s="16"/>
-      <c r="AF83" s="16"/>
-      <c r="AG83" s="17"/>
+      <c r="B83" s="20"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="20"/>
+      <c r="E83" s="20"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="20"/>
+      <c r="H83" s="20"/>
+      <c r="I83" s="20"/>
+      <c r="J83" s="20"/>
+      <c r="K83" s="20"/>
+      <c r="L83" s="20"/>
+      <c r="M83" s="20"/>
+      <c r="N83" s="20"/>
+      <c r="O83" s="20"/>
+      <c r="P83" s="20"/>
+      <c r="Q83" s="20"/>
+      <c r="R83" s="20"/>
+      <c r="S83" s="20"/>
+      <c r="T83" s="20"/>
+      <c r="U83" s="20"/>
+      <c r="V83" s="20"/>
+      <c r="W83" s="20"/>
+      <c r="X83" s="20"/>
+      <c r="Y83" s="20"/>
+      <c r="Z83" s="20"/>
+      <c r="AA83" s="20"/>
+      <c r="AB83" s="20"/>
+      <c r="AC83" s="20"/>
+      <c r="AD83" s="20"/>
+      <c r="AE83" s="20"/>
+      <c r="AF83" s="20"/>
+      <c r="AG83" s="21"/>
     </row>
     <row r="84" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A84" s="18" t="s">
+      <c r="A84" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B84" s="19"/>
-      <c r="C84" s="19"/>
-      <c r="D84" s="19"/>
-      <c r="E84" s="19"/>
-      <c r="F84" s="19"/>
-      <c r="G84" s="19"/>
-      <c r="H84" s="19"/>
-      <c r="I84" s="19"/>
-      <c r="J84" s="19"/>
-      <c r="K84" s="19"/>
-      <c r="L84" s="19"/>
-      <c r="M84" s="19"/>
-      <c r="N84" s="19"/>
-      <c r="O84" s="19"/>
-      <c r="P84" s="19"/>
-      <c r="Q84" s="19"/>
-      <c r="R84" s="19"/>
-      <c r="S84" s="19"/>
-      <c r="T84" s="19"/>
-      <c r="U84" s="19"/>
-      <c r="V84" s="19"/>
-      <c r="W84" s="19"/>
-      <c r="X84" s="19"/>
-      <c r="Y84" s="19"/>
-      <c r="Z84" s="19"/>
-      <c r="AA84" s="19"/>
-      <c r="AB84" s="19"/>
-      <c r="AC84" s="19"/>
-      <c r="AD84" s="19"/>
-      <c r="AE84" s="19"/>
-      <c r="AF84" s="19"/>
-      <c r="AG84" s="20"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="13"/>
+      <c r="L84" s="13"/>
+      <c r="M84" s="13"/>
+      <c r="N84" s="13"/>
+      <c r="O84" s="13"/>
+      <c r="P84" s="13"/>
+      <c r="Q84" s="13"/>
+      <c r="R84" s="13"/>
+      <c r="S84" s="13"/>
+      <c r="T84" s="13"/>
+      <c r="U84" s="13"/>
+      <c r="V84" s="13"/>
+      <c r="W84" s="13"/>
+      <c r="X84" s="13"/>
+      <c r="Y84" s="13"/>
+      <c r="Z84" s="13"/>
+      <c r="AA84" s="13"/>
+      <c r="AB84" s="13"/>
+      <c r="AC84" s="13"/>
+      <c r="AD84" s="13"/>
+      <c r="AE84" s="13"/>
+      <c r="AF84" s="13"/>
+      <c r="AG84" s="14"/>
     </row>
     <row r="85" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
@@ -11920,41 +11855,41 @@
       </c>
     </row>
     <row r="91" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A91" s="12" t="s">
+      <c r="A91" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B91" s="13"/>
-      <c r="C91" s="13"/>
-      <c r="D91" s="13"/>
-      <c r="E91" s="13"/>
-      <c r="F91" s="13"/>
-      <c r="G91" s="13"/>
-      <c r="H91" s="13"/>
-      <c r="I91" s="13"/>
-      <c r="J91" s="13"/>
-      <c r="K91" s="13"/>
-      <c r="L91" s="13"/>
-      <c r="M91" s="13"/>
-      <c r="N91" s="13"/>
-      <c r="O91" s="13"/>
-      <c r="P91" s="13"/>
-      <c r="Q91" s="13"/>
-      <c r="R91" s="13"/>
-      <c r="S91" s="13"/>
-      <c r="T91" s="13"/>
-      <c r="U91" s="13"/>
-      <c r="V91" s="13"/>
-      <c r="W91" s="13"/>
-      <c r="X91" s="13"/>
-      <c r="Y91" s="13"/>
-      <c r="Z91" s="13"/>
-      <c r="AA91" s="13"/>
-      <c r="AB91" s="13"/>
-      <c r="AC91" s="13"/>
-      <c r="AD91" s="13"/>
-      <c r="AE91" s="13"/>
-      <c r="AF91" s="13"/>
-      <c r="AG91" s="14"/>
+      <c r="B91" s="16"/>
+      <c r="C91" s="16"/>
+      <c r="D91" s="16"/>
+      <c r="E91" s="16"/>
+      <c r="F91" s="16"/>
+      <c r="G91" s="16"/>
+      <c r="H91" s="16"/>
+      <c r="I91" s="16"/>
+      <c r="J91" s="16"/>
+      <c r="K91" s="16"/>
+      <c r="L91" s="16"/>
+      <c r="M91" s="16"/>
+      <c r="N91" s="16"/>
+      <c r="O91" s="16"/>
+      <c r="P91" s="16"/>
+      <c r="Q91" s="16"/>
+      <c r="R91" s="16"/>
+      <c r="S91" s="16"/>
+      <c r="T91" s="16"/>
+      <c r="U91" s="16"/>
+      <c r="V91" s="16"/>
+      <c r="W91" s="16"/>
+      <c r="X91" s="16"/>
+      <c r="Y91" s="16"/>
+      <c r="Z91" s="16"/>
+      <c r="AA91" s="16"/>
+      <c r="AB91" s="16"/>
+      <c r="AC91" s="16"/>
+      <c r="AD91" s="16"/>
+      <c r="AE91" s="16"/>
+      <c r="AF91" s="16"/>
+      <c r="AG91" s="17"/>
     </row>
     <row r="92" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>

</xml_diff>